<commit_message>
Finalización del calendario de pesos para empleados
</commit_message>
<xml_diff>
--- a/parser/Empleados.xlsx
+++ b/parser/Empleados.xlsx
@@ -297,10 +297,10 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -526,17 +526,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -564,10 +564,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Georgia"/>
-            <a:ea typeface="Georgia"/>
-            <a:cs typeface="Georgia"/>
-            <a:sym typeface="Georgia"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -815,12 +815,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1107,7 +1107,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1135,10 +1135,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Georgia"/>
-            <a:ea typeface="Georgia"/>
-            <a:cs typeface="Georgia"/>
-            <a:sym typeface="Georgia"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1534,10 +1534,10 @@
         <v>1</v>
       </c>
       <c r="S2" s="6">
-        <v>49</v>
+        <v>-1</v>
       </c>
       <c r="T2" s="6">
-        <v>49</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -1658,10 +1658,10 @@
         <v>1</v>
       </c>
       <c r="S4" s="6">
-        <v>49</v>
+        <v>-1</v>
       </c>
       <c r="T4" s="6">
-        <v>49</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">

</xml_diff>